<commit_message>
Updated sales logic with charts
</commit_message>
<xml_diff>
--- a/data/processed/car-sales-output.xlsx
+++ b/data/processed/car-sales-output.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,883 +437,1038 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>months</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Car Model</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Non Taxable Amount</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CGST 9 %</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>SGST 9 %</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total Sale</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Total Tax</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Total Sale</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Januray</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Swift LXI</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>2500000</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>450000</v>
       </c>
       <c r="F2" t="n">
         <v>450000</v>
       </c>
       <c r="G2" t="n">
-        <v>900000</v>
+        <v>450000</v>
       </c>
       <c r="H2" t="n">
         <v>5900000</v>
       </c>
+      <c r="I2" t="n">
+        <v>900000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Februrary</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Swift VXI</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>1500000</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>3000000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>270000</v>
       </c>
       <c r="F3" t="n">
         <v>270000</v>
       </c>
       <c r="G3" t="n">
-        <v>540000</v>
+        <v>270000</v>
       </c>
       <c r="H3" t="n">
         <v>3540000</v>
       </c>
+      <c r="I3" t="n">
+        <v>540000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Swift ZXI</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>2000000</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>8000000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>720000</v>
       </c>
       <c r="F4" t="n">
         <v>720000</v>
       </c>
       <c r="G4" t="n">
-        <v>1440000</v>
+        <v>720000</v>
       </c>
       <c r="H4" t="n">
         <v>9440000</v>
       </c>
+      <c r="I4" t="n">
+        <v>1440000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Baleno Sigma</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>3000000</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>9000000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>810000</v>
       </c>
       <c r="F5" t="n">
         <v>810000</v>
       </c>
       <c r="G5" t="n">
-        <v>1620000</v>
+        <v>810000</v>
       </c>
       <c r="H5" t="n">
         <v>10620000</v>
       </c>
+      <c r="I5" t="n">
+        <v>1620000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>Baleno Delta</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>4100000</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>8200000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>738000</v>
       </c>
       <c r="F6" t="n">
         <v>738000</v>
       </c>
       <c r="G6" t="n">
-        <v>1476000</v>
+        <v>738000</v>
       </c>
       <c r="H6" t="n">
         <v>9676000</v>
       </c>
+      <c r="I6" t="n">
+        <v>1476000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Baleno Alpha</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2300000</v>
       </c>
       <c r="D7" t="n">
         <v>2300000</v>
       </c>
       <c r="E7" t="n">
-        <v>207000</v>
+        <v>2300000</v>
       </c>
       <c r="F7" t="n">
         <v>207000</v>
       </c>
       <c r="G7" t="n">
-        <v>414000</v>
+        <v>207000</v>
       </c>
       <c r="H7" t="n">
         <v>2714000</v>
       </c>
+      <c r="I7" t="n">
+        <v>414000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>August</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Alto 800 STD</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>4</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>3800000</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>15200000</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1368000</v>
       </c>
       <c r="F8" t="n">
         <v>1368000</v>
       </c>
       <c r="G8" t="n">
-        <v>2736000</v>
+        <v>1368000</v>
       </c>
       <c r="H8" t="n">
         <v>17936000</v>
       </c>
+      <c r="I8" t="n">
+        <v>2736000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>Alto 800 LXI</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>2</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>4200000</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>8400000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>756000</v>
       </c>
       <c r="F9" t="n">
         <v>756000</v>
       </c>
       <c r="G9" t="n">
-        <v>1512000</v>
+        <v>756000</v>
       </c>
       <c r="H9" t="n">
         <v>9912000</v>
       </c>
+      <c r="I9" t="n">
+        <v>1512000</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>WagonR LXI</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>2</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>6000000</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>12000000</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1080000</v>
       </c>
       <c r="F10" t="n">
         <v>1080000</v>
       </c>
       <c r="G10" t="n">
-        <v>2160000</v>
+        <v>1080000</v>
       </c>
       <c r="H10" t="n">
         <v>14160000</v>
       </c>
+      <c r="I10" t="n">
+        <v>2160000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>WagonR VXI</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>1</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1650000</v>
       </c>
       <c r="D11" t="n">
         <v>1650000</v>
       </c>
       <c r="E11" t="n">
-        <v>148500</v>
+        <v>1650000</v>
       </c>
       <c r="F11" t="n">
         <v>148500</v>
       </c>
       <c r="G11" t="n">
-        <v>297000</v>
+        <v>148500</v>
       </c>
       <c r="H11" t="n">
         <v>1947000</v>
       </c>
+      <c r="I11" t="n">
+        <v>297000</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>WagonR ZXI</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>6</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>1690000</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>10140000</v>
-      </c>
-      <c r="E12" t="n">
-        <v>912600</v>
       </c>
       <c r="F12" t="n">
         <v>912600</v>
       </c>
       <c r="G12" t="n">
-        <v>1825200</v>
+        <v>912600</v>
       </c>
       <c r="H12" t="n">
         <v>11965200</v>
       </c>
+      <c r="I12" t="n">
+        <v>1825200</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Decenber</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>Dzire LX</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>4</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>1690000</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>6760000</v>
-      </c>
-      <c r="E13" t="n">
-        <v>608400</v>
       </c>
       <c r="F13" t="n">
         <v>608400</v>
       </c>
       <c r="G13" t="n">
-        <v>1216800</v>
+        <v>608400</v>
       </c>
       <c r="H13" t="n">
         <v>7976800</v>
       </c>
+      <c r="I13" t="n">
+        <v>1216800</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>Dzire VXI</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1760000</v>
       </c>
       <c r="D14" t="n">
         <v>1760000</v>
       </c>
       <c r="E14" t="n">
-        <v>158400</v>
+        <v>1760000</v>
       </c>
       <c r="F14" t="n">
         <v>158400</v>
       </c>
       <c r="G14" t="n">
-        <v>316800</v>
+        <v>158400</v>
       </c>
       <c r="H14" t="n">
         <v>2076800</v>
       </c>
+      <c r="I14" t="n">
+        <v>316800</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>Dzire ZXI</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>6</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>1860000</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>11160000</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1004400</v>
       </c>
       <c r="F15" t="n">
         <v>1004400</v>
       </c>
       <c r="G15" t="n">
-        <v>2008800</v>
+        <v>1004400</v>
       </c>
       <c r="H15" t="n">
         <v>13168800</v>
       </c>
+      <c r="I15" t="n">
+        <v>2008800</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>Brezza VXI</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1980000</v>
       </c>
       <c r="D16" t="n">
         <v>1980000</v>
       </c>
       <c r="E16" t="n">
-        <v>178200</v>
+        <v>1980000</v>
       </c>
       <c r="F16" t="n">
         <v>178200</v>
       </c>
       <c r="G16" t="n">
-        <v>356400</v>
+        <v>178200</v>
       </c>
       <c r="H16" t="n">
         <v>2336400</v>
       </c>
+      <c r="I16" t="n">
+        <v>356400</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>Brezza ZXI</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="C17" t="n">
         <v>7</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>1150000</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>8050000</v>
-      </c>
-      <c r="E17" t="n">
-        <v>724500</v>
       </c>
       <c r="F17" t="n">
         <v>724500</v>
       </c>
       <c r="G17" t="n">
-        <v>1449000</v>
+        <v>724500</v>
       </c>
       <c r="H17" t="n">
         <v>9499000</v>
       </c>
+      <c r="I17" t="n">
+        <v>1449000</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Februrary</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Ertiga VXI</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="C18" t="n">
         <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1050000</v>
       </c>
       <c r="D18" t="n">
         <v>1050000</v>
       </c>
       <c r="E18" t="n">
-        <v>94500</v>
+        <v>1050000</v>
       </c>
       <c r="F18" t="n">
         <v>94500</v>
       </c>
       <c r="G18" t="n">
-        <v>189000</v>
+        <v>94500</v>
       </c>
       <c r="H18" t="n">
         <v>1239000</v>
       </c>
+      <c r="I18" t="n">
+        <v>189000</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>Ertiga ZXI</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="C19" t="n">
         <v>2</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>1250000</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>2500000</v>
-      </c>
-      <c r="E19" t="n">
-        <v>225000</v>
       </c>
       <c r="F19" t="n">
         <v>225000</v>
       </c>
       <c r="G19" t="n">
-        <v>450000</v>
+        <v>225000</v>
       </c>
       <c r="H19" t="n">
         <v>2950000</v>
       </c>
+      <c r="I19" t="n">
+        <v>450000</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>Eeco Cargo</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="C20" t="n">
         <v>3</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>5400000</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>16200000</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1458000</v>
       </c>
       <c r="F20" t="n">
         <v>1458000</v>
       </c>
       <c r="G20" t="n">
-        <v>2916000</v>
+        <v>1458000</v>
       </c>
       <c r="H20" t="n">
         <v>19116000</v>
       </c>
+      <c r="I20" t="n">
+        <v>2916000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Decenber</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>Eeco Passenger</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="C21" t="n">
         <v>2</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>5800000</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>11600000</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1044000</v>
       </c>
       <c r="F21" t="n">
         <v>1044000</v>
       </c>
       <c r="G21" t="n">
-        <v>2088000</v>
+        <v>1044000</v>
       </c>
       <c r="H21" t="n">
         <v>13688000</v>
       </c>
+      <c r="I21" t="n">
+        <v>2088000</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>August</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>Celerio LXI</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="C22" t="n">
         <v>2</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>6100000</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>12200000</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1098000</v>
       </c>
       <c r="F22" t="n">
         <v>1098000</v>
       </c>
       <c r="G22" t="n">
-        <v>2196000</v>
+        <v>1098000</v>
       </c>
       <c r="H22" t="n">
         <v>14396000</v>
       </c>
+      <c r="I22" t="n">
+        <v>2196000</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>Celerio ZXI</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="C23" t="n">
         <v>1</v>
-      </c>
-      <c r="C23" t="n">
-        <v>6900000</v>
       </c>
       <c r="D23" t="n">
         <v>6900000</v>
       </c>
       <c r="E23" t="n">
-        <v>621000</v>
+        <v>6900000</v>
       </c>
       <c r="F23" t="n">
         <v>621000</v>
       </c>
       <c r="G23" t="n">
-        <v>1242000</v>
+        <v>621000</v>
       </c>
       <c r="H23" t="n">
         <v>8142000</v>
       </c>
+      <c r="I23" t="n">
+        <v>1242000</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>September</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>Ignis Sigma</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="C24" t="n">
         <v>5</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>6200000</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>31000000</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2790000</v>
       </c>
       <c r="F24" t="n">
         <v>2790000</v>
       </c>
       <c r="G24" t="n">
-        <v>5580000</v>
+        <v>2790000</v>
       </c>
       <c r="H24" t="n">
         <v>36580000</v>
       </c>
+      <c r="I24" t="n">
+        <v>5580000</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Decenber</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>Ignis Alpha</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="C25" t="n">
         <v>1</v>
-      </c>
-      <c r="C25" t="n">
-        <v>8200000</v>
       </c>
       <c r="D25" t="n">
         <v>8200000</v>
       </c>
       <c r="E25" t="n">
-        <v>738000</v>
+        <v>8200000</v>
       </c>
       <c r="F25" t="n">
         <v>738000</v>
       </c>
       <c r="G25" t="n">
-        <v>1476000</v>
+        <v>738000</v>
       </c>
       <c r="H25" t="n">
         <v>9676000</v>
       </c>
+      <c r="I25" t="n">
+        <v>1476000</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>XL6 Zeta</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="C26" t="n">
         <v>3</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>1150000</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>3450000</v>
-      </c>
-      <c r="E26" t="n">
-        <v>310500</v>
       </c>
       <c r="F26" t="n">
         <v>310500</v>
       </c>
       <c r="G26" t="n">
-        <v>621000</v>
+        <v>310500</v>
       </c>
       <c r="H26" t="n">
         <v>4071000</v>
       </c>
+      <c r="I26" t="n">
+        <v>621000</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>XL6 Alpha</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="C27" t="n">
         <v>1</v>
-      </c>
-      <c r="C27" t="n">
-        <v>3000000</v>
       </c>
       <c r="D27" t="n">
         <v>3000000</v>
       </c>
       <c r="E27" t="n">
-        <v>270000</v>
+        <v>3000000</v>
       </c>
       <c r="F27" t="n">
         <v>270000</v>
       </c>
       <c r="G27" t="n">
-        <v>540000</v>
+        <v>270000</v>
       </c>
       <c r="H27" t="n">
         <v>3540000</v>
       </c>
+      <c r="I27" t="n">
+        <v>540000</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>September</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>Fronx Delta</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="C28" t="n">
         <v>2</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>8800000</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>17600000</v>
-      </c>
-      <c r="E28" t="n">
-        <v>1584000</v>
       </c>
       <c r="F28" t="n">
         <v>1584000</v>
       </c>
       <c r="G28" t="n">
-        <v>3168000</v>
+        <v>1584000</v>
       </c>
       <c r="H28" t="n">
         <v>20768000</v>
       </c>
+      <c r="I28" t="n">
+        <v>3168000</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>Fronx Alpha</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="C29" t="n">
         <v>2</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>1120000</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>2240000</v>
-      </c>
-      <c r="E29" t="n">
-        <v>201600</v>
       </c>
       <c r="F29" t="n">
         <v>201600</v>
       </c>
       <c r="G29" t="n">
-        <v>403200</v>
+        <v>201600</v>
       </c>
       <c r="H29" t="n">
         <v>2643200</v>
       </c>
+      <c r="I29" t="n">
+        <v>403200</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>Jimny Zeta</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="C30" t="n">
         <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1250000</v>
       </c>
       <c r="D30" t="n">
         <v>1250000</v>
       </c>
       <c r="E30" t="n">
-        <v>112500</v>
+        <v>1250000</v>
       </c>
       <c r="F30" t="n">
         <v>112500</v>
       </c>
       <c r="G30" t="n">
-        <v>225000</v>
+        <v>112500</v>
       </c>
       <c r="H30" t="n">
         <v>1475000</v>
       </c>
+      <c r="I30" t="n">
+        <v>225000</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>januray</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>Jimny Alpha</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="C31" t="n">
         <v>8</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>1450000</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>11600000</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1044000</v>
       </c>
       <c r="F31" t="n">
         <v>1044000</v>
       </c>
       <c r="G31" t="n">
-        <v>2088000</v>
+        <v>1044000</v>
       </c>
       <c r="H31" t="n">
         <v>13688000</v>
+      </c>
+      <c r="I31" t="n">
+        <v>2088000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>